<commit_message>
implemented 1-1 correlations while also using PCA
</commit_message>
<xml_diff>
--- a/cleaning_notebook/AB_cleaned_formatted.xlsx
+++ b/cleaning_notebook/AB_cleaned_formatted.xlsx
@@ -804,7 +804,7 @@
         <v>96.90000000000001</v>
       </c>
       <c r="AU2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:47">
@@ -947,7 +947,7 @@
         <v>99.7</v>
       </c>
       <c r="AU3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:47">
@@ -1090,7 +1090,7 @@
         <v>139.1</v>
       </c>
       <c r="AU4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:47">
@@ -1233,7 +1233,7 @@
         <v>125.1</v>
       </c>
       <c r="AU5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:47">
@@ -1376,7 +1376,7 @@
         <v>134.5</v>
       </c>
       <c r="AU6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:47">
@@ -1519,7 +1519,7 @@
         <v>94.40000000000001</v>
       </c>
       <c r="AU7">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:47">
@@ -1662,7 +1662,7 @@
         <v>106.2</v>
       </c>
       <c r="AU8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:47">
@@ -1805,7 +1805,7 @@
         <v>97.90000000000001</v>
       </c>
       <c r="AU9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -1948,7 +1948,7 @@
         <v>100.8</v>
       </c>
       <c r="AU10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -2091,7 +2091,7 @@
         <v>97.3</v>
       </c>
       <c r="AU11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:47">
@@ -2234,7 +2234,7 @@
         <v>94.7</v>
       </c>
       <c r="AU12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:47">
@@ -2377,7 +2377,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:47">
@@ -2520,7 +2520,7 @@
         <v>105.6</v>
       </c>
       <c r="AU14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:47">
@@ -2663,7 +2663,7 @@
         <v>120.6</v>
       </c>
       <c r="AU15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:47">
@@ -2806,7 +2806,7 @@
         <v>137.5</v>
       </c>
       <c r="AU16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:47">
@@ -2949,7 +2949,7 @@
         <v>118.7</v>
       </c>
       <c r="AU17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:47">
@@ -3092,7 +3092,7 @@
         <v>98.09999999999999</v>
       </c>
       <c r="AU18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:47">
@@ -3235,7 +3235,7 @@
         <v>113.6</v>
       </c>
       <c r="AU19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:47">
@@ -3378,7 +3378,7 @@
         <v>104.2</v>
       </c>
       <c r="AU20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:47">
@@ -3521,7 +3521,7 @@
         <v>106.8</v>
       </c>
       <c r="AU21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:47">
@@ -3664,7 +3664,7 @@
         <v>122.1</v>
       </c>
       <c r="AU22">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:47">
@@ -3807,7 +3807,7 @@
         <v>105.1</v>
       </c>
       <c r="AU23">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:47">
@@ -3950,7 +3950,7 @@
         <v>97.3</v>
       </c>
       <c r="AU24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:47">
@@ -4093,7 +4093,7 @@
         <v>142.1</v>
       </c>
       <c r="AU25">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:47">
@@ -4236,7 +4236,7 @@
         <v>119.9</v>
       </c>
       <c r="AU26">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:47">
@@ -4379,7 +4379,7 @@
         <v>145.7</v>
       </c>
       <c r="AU27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:47">
@@ -4522,7 +4522,7 @@
         <v>139.7</v>
       </c>
       <c r="AU28">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:47">
@@ -4665,7 +4665,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU29">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:47">
@@ -4808,7 +4808,7 @@
         <v>100.3</v>
       </c>
       <c r="AU30">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:47">
@@ -4951,7 +4951,7 @@
         <v>125.8</v>
       </c>
       <c r="AU31">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:47">
@@ -5094,7 +5094,7 @@
         <v>109.1</v>
       </c>
       <c r="AU32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:47">
@@ -5237,7 +5237,7 @@
         <v>138.4</v>
       </c>
       <c r="AU33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:47">
@@ -5380,7 +5380,7 @@
         <v>124.1</v>
       </c>
       <c r="AU34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:47">
@@ -5523,7 +5523,7 @@
         <v>154.8</v>
       </c>
       <c r="AU35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:47">
@@ -5666,7 +5666,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU36">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:47">
@@ -5809,7 +5809,7 @@
         <v>113.3</v>
       </c>
       <c r="AU37">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:47">
@@ -5952,7 +5952,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU38">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:47">
@@ -6095,7 +6095,7 @@
         <v>107.1</v>
       </c>
       <c r="AU39">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:47">
@@ -6238,7 +6238,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU40">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:47">
@@ -6381,7 +6381,7 @@
         <v>116.6</v>
       </c>
       <c r="AU41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:47">
@@ -6524,7 +6524,7 @@
         <v>109</v>
       </c>
       <c r="AU42">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:47">
@@ -6667,7 +6667,7 @@
         <v>61</v>
       </c>
       <c r="AU43">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:47">
@@ -6810,7 +6810,7 @@
         <v>140.3</v>
       </c>
       <c r="AU44">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:47">
@@ -6953,7 +6953,7 @@
         <v>109</v>
       </c>
       <c r="AU45">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:47">
@@ -7096,7 +7096,7 @@
         <v>123.6</v>
       </c>
       <c r="AU46">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:47">
@@ -7239,7 +7239,7 @@
         <v>113.7</v>
       </c>
       <c r="AU47">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:47">
@@ -7382,7 +7382,7 @@
         <v>117.5</v>
       </c>
       <c r="AU48">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:47">
@@ -7525,7 +7525,7 @@
         <v>97.3</v>
       </c>
       <c r="AU49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:47">
@@ -7668,7 +7668,7 @@
         <v>119.7</v>
       </c>
       <c r="AU50">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:47">
@@ -7811,7 +7811,7 @@
         <v>81.40000000000001</v>
       </c>
       <c r="AU51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:47">
@@ -7954,7 +7954,7 @@
         <v>106.7</v>
       </c>
       <c r="AU52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:47">
@@ -8097,7 +8097,7 @@
         <v>141.5</v>
       </c>
       <c r="AU53">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:47">
@@ -8240,7 +8240,7 @@
         <v>114.5</v>
       </c>
       <c r="AU54">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:47">
@@ -8383,7 +8383,7 @@
         <v>98.09999999999999</v>
       </c>
       <c r="AU55">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:47">
@@ -8526,7 +8526,7 @@
         <v>107.2</v>
       </c>
       <c r="AU56">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:47">
@@ -8669,7 +8669,7 @@
         <v>120.8</v>
       </c>
       <c r="AU57">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:47">
@@ -8812,7 +8812,7 @@
         <v>103.7</v>
       </c>
       <c r="AU58">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:47">
@@ -8955,7 +8955,7 @@
         <v>91.09999999999999</v>
       </c>
       <c r="AU59">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:47">
@@ -9098,7 +9098,7 @@
         <v>79.8</v>
       </c>
       <c r="AU60">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:47">
@@ -9241,7 +9241,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU61">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:47">
@@ -9384,7 +9384,7 @@
         <v>103.3</v>
       </c>
       <c r="AU62">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:47">
@@ -9527,7 +9527,7 @@
         <v>91.7</v>
       </c>
       <c r="AU63">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:47">
@@ -9670,7 +9670,7 @@
         <v>108.2</v>
       </c>
       <c r="AU64">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:47">
@@ -9813,7 +9813,7 @@
         <v>95.2</v>
       </c>
       <c r="AU65">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:47">
@@ -9956,7 +9956,7 @@
         <v>112.8</v>
       </c>
       <c r="AU66">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:47">
@@ -10099,7 +10099,7 @@
         <v>112.1</v>
       </c>
       <c r="AU67">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:47">
@@ -10242,7 +10242,7 @@
         <v>91.3</v>
       </c>
       <c r="AU68">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:47">
@@ -10385,7 +10385,7 @@
         <v>96.40000000000001</v>
       </c>
       <c r="AU69">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:47">
@@ -10528,7 +10528,7 @@
         <v>126.1</v>
       </c>
       <c r="AU70">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:47">
@@ -10671,7 +10671,7 @@
         <v>97.5</v>
       </c>
       <c r="AU71">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:47">
@@ -10814,7 +10814,7 @@
         <v>130.2</v>
       </c>
       <c r="AU72">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:47">
@@ -10957,7 +10957,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU73">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:47">
@@ -11100,7 +11100,7 @@
         <v>111.8</v>
       </c>
       <c r="AU74">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:47">
@@ -11243,7 +11243,7 @@
         <v>84</v>
       </c>
       <c r="AU75">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:47">
@@ -11386,7 +11386,7 @@
         <v>86.7</v>
       </c>
       <c r="AU76">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:47">
@@ -11529,7 +11529,7 @@
         <v>89.59999999999999</v>
       </c>
       <c r="AU77">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:47">
@@ -11672,7 +11672,7 @@
         <v>115.7</v>
       </c>
       <c r="AU78">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:47">
@@ -11815,7 +11815,7 @@
         <v>99</v>
       </c>
       <c r="AU79">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:47">
@@ -11958,7 +11958,7 @@
         <v>157.3</v>
       </c>
       <c r="AU80">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:47">
@@ -12101,7 +12101,7 @@
         <v>132.2</v>
       </c>
       <c r="AU81">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:47">
@@ -12244,7 +12244,7 @@
         <v>108.2</v>
       </c>
       <c r="AU82">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:47">
@@ -12387,7 +12387,7 @@
         <v>98</v>
       </c>
       <c r="AU83">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:47">
@@ -12530,7 +12530,7 @@
         <v>96.59999999999999</v>
       </c>
       <c r="AU84">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:47">
@@ -12673,7 +12673,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU85">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:47">
@@ -12816,7 +12816,7 @@
         <v>160.7</v>
       </c>
       <c r="AU86">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:47">
@@ -12959,7 +12959,7 @@
         <v>108.3</v>
       </c>
       <c r="AU87">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:47">
@@ -13102,7 +13102,7 @@
         <v>108.2</v>
       </c>
       <c r="AU88">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:47">
@@ -13245,7 +13245,7 @@
         <v>101.1</v>
       </c>
       <c r="AU89">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:47">
@@ -13388,7 +13388,7 @@
         <v>112.2</v>
       </c>
       <c r="AU90">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:47">
@@ -13531,7 +13531,7 @@
         <v>112</v>
       </c>
       <c r="AU91">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:47">
@@ -13674,7 +13674,7 @@
         <v>101.8</v>
       </c>
       <c r="AU92">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:47">
@@ -13817,7 +13817,7 @@
         <v>97.3</v>
       </c>
       <c r="AU93">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:47">
@@ -13960,7 +13960,7 @@
         <v>85</v>
       </c>
       <c r="AU94">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:47">
@@ -14103,7 +14103,7 @@
         <v>83.2</v>
       </c>
       <c r="AU95">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:47">
@@ -14246,7 +14246,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU96">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:47">
@@ -14389,7 +14389,7 @@
         <v>99.8</v>
       </c>
       <c r="AU97">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:47">
@@ -14532,7 +14532,7 @@
         <v>137.2</v>
       </c>
       <c r="AU98">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:47">
@@ -14675,7 +14675,7 @@
         <v>122.9</v>
       </c>
       <c r="AU99">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:47">
@@ -14818,7 +14818,7 @@
         <v>97</v>
       </c>
       <c r="AU100">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:47">
@@ -14961,7 +14961,7 @@
         <v>91.90000000000001</v>
       </c>
       <c r="AU101">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:47">
@@ -15104,7 +15104,7 @@
         <v>105.4</v>
       </c>
       <c r="AU102">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:47">
@@ -15247,7 +15247,7 @@
         <v>124.2</v>
       </c>
       <c r="AU103">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:47">
@@ -15390,7 +15390,7 @@
         <v>99.3</v>
       </c>
       <c r="AU104">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:47">
@@ -15533,7 +15533,7 @@
         <v>77.90000000000001</v>
       </c>
       <c r="AU105">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:47">
@@ -15676,7 +15676,7 @@
         <v>97.8</v>
       </c>
       <c r="AU106">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:47">
@@ -15819,7 +15819,7 @@
         <v>110.2</v>
       </c>
       <c r="AU107">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:47">
@@ -15962,7 +15962,7 @@
         <v>114.4</v>
       </c>
       <c r="AU108">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:47">
@@ -16105,7 +16105,7 @@
         <v>124.1</v>
       </c>
       <c r="AU109">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:47">
@@ -16248,7 +16248,7 @@
         <v>109.8</v>
       </c>
       <c r="AU110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:47">
@@ -16391,7 +16391,7 @@
         <v>97.90000000000001</v>
       </c>
       <c r="AU111">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:47">
@@ -16534,7 +16534,7 @@
         <v>96</v>
       </c>
       <c r="AU112">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:47">
@@ -16677,7 +16677,7 @@
         <v>92.90000000000001</v>
       </c>
       <c r="AU113">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:47">
@@ -16820,7 +16820,7 @@
         <v>104</v>
       </c>
       <c r="AU114">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:47">
@@ -16963,7 +16963,7 @@
         <v>88.09999999999999</v>
       </c>
       <c r="AU115">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:47">
@@ -17106,7 +17106,7 @@
         <v>145.8</v>
       </c>
       <c r="AU116">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:47">
@@ -17249,7 +17249,7 @@
         <v>91.8</v>
       </c>
       <c r="AU117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:47">
@@ -17392,7 +17392,7 @@
         <v>137.7</v>
       </c>
       <c r="AU118">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:47">
@@ -17535,7 +17535,7 @@
         <v>100.5</v>
       </c>
       <c r="AU119">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:47">
@@ -17678,7 +17678,7 @@
         <v>106.7</v>
       </c>
       <c r="AU120">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:47">
@@ -17821,7 +17821,7 @@
         <v>136.3</v>
       </c>
       <c r="AU121">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:47">
@@ -17964,7 +17964,7 @@
         <v>133.2</v>
       </c>
       <c r="AU122">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:47">
@@ -18107,7 +18107,7 @@
         <v>118.4</v>
       </c>
       <c r="AU123">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:47">
@@ -18250,7 +18250,7 @@
         <v>81.40000000000001</v>
       </c>
       <c r="AU124">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:47">
@@ -18393,7 +18393,7 @@
         <v>115.8</v>
       </c>
       <c r="AU125">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:47">
@@ -18536,7 +18536,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU126">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:47">
@@ -18679,7 +18679,7 @@
         <v>107.9</v>
       </c>
       <c r="AU127">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:47">
@@ -18822,7 +18822,7 @@
         <v>91.8</v>
       </c>
       <c r="AU128">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:47">
@@ -18965,7 +18965,7 @@
         <v>109.9</v>
       </c>
       <c r="AU129">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:47">
@@ -19108,7 +19108,7 @@
         <v>101</v>
       </c>
       <c r="AU130">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:47">
@@ -19251,7 +19251,7 @@
         <v>87</v>
       </c>
       <c r="AU131">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:47">
@@ -19394,7 +19394,7 @@
         <v>95.59999999999999</v>
       </c>
       <c r="AU132">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:47">
@@ -19537,7 +19537,7 @@
         <v>79.40000000000001</v>
       </c>
       <c r="AU133">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:47">
@@ -19680,7 +19680,7 @@
         <v>88.40000000000001</v>
       </c>
       <c r="AU134">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:47">
@@ -19823,7 +19823,7 @@
         <v>98.59999999999999</v>
       </c>
       <c r="AU135">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:47">
@@ -19966,7 +19966,7 @@
         <v>84</v>
       </c>
       <c r="AU136">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:47">
@@ -20109,7 +20109,7 @@
         <v>97.09999999999999</v>
       </c>
       <c r="AU137">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:47">
@@ -20252,7 +20252,7 @@
         <v>95.2</v>
       </c>
       <c r="AU138">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:47">
@@ -20395,7 +20395,7 @@
         <v>116.3</v>
       </c>
       <c r="AU139">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:47">
@@ -20538,7 +20538,7 @@
         <v>95.59999999999999</v>
       </c>
       <c r="AU140">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:47">
@@ -20681,7 +20681,7 @@
         <v>91.90000000000001</v>
       </c>
       <c r="AU141">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:47">
@@ -20824,7 +20824,7 @@
         <v>128.5</v>
       </c>
       <c r="AU142">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:47">
@@ -20967,7 +20967,7 @@
         <v>106.5</v>
       </c>
       <c r="AU143">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:47">
@@ -21110,7 +21110,7 @@
         <v>128</v>
       </c>
       <c r="AU144">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:47">
@@ -21253,7 +21253,7 @@
         <v>92.3</v>
       </c>
       <c r="AU145">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:47">
@@ -21396,7 +21396,7 @@
         <v>117.1</v>
       </c>
       <c r="AU146">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:47">
@@ -21539,7 +21539,7 @@
         <v>91.8</v>
       </c>
       <c r="AU147">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:47">
@@ -21682,7 +21682,7 @@
         <v>108.8762987012987</v>
       </c>
       <c r="AU148">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:47">
@@ -21825,7 +21825,7 @@
         <v>109.6</v>
       </c>
       <c r="AU149">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:47">
@@ -21968,7 +21968,7 @@
         <v>124.1</v>
       </c>
       <c r="AU150">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:47">
@@ -22111,7 +22111,7 @@
         <v>89.40000000000001</v>
       </c>
       <c r="AU151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:47">
@@ -22254,7 +22254,7 @@
         <v>131.6</v>
       </c>
       <c r="AU152">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:47">
@@ -22397,7 +22397,7 @@
         <v>80.90000000000001</v>
       </c>
       <c r="AU153">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:47">
@@ -22540,7 +22540,7 @@
         <v>142.1</v>
       </c>
       <c r="AU154">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:47">
@@ -22683,7 +22683,7 @@
         <v>92.40000000000001</v>
       </c>
       <c r="AU155">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:47">
@@ -22826,7 +22826,7 @@
         <v>87.8</v>
       </c>
       <c r="AU156">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:47">
@@ -22969,7 +22969,7 @@
         <v>114.9</v>
       </c>
       <c r="AU157">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:47">
@@ -23112,7 +23112,7 @@
         <v>97.5</v>
       </c>
       <c r="AU158">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:47">
@@ -23255,7 +23255,7 @@
         <v>128</v>
       </c>
       <c r="AU159">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:47">
@@ -23398,7 +23398,7 @@
         <v>103.9</v>
       </c>
       <c r="AU160">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:47">
@@ -23541,7 +23541,7 @@
         <v>121.9</v>
       </c>
       <c r="AU161">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:47">
@@ -23684,7 +23684,7 @@
         <v>97.7</v>
       </c>
       <c r="AU162">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:47">
@@ -23827,7 +23827,7 @@
         <v>86.8</v>
       </c>
       <c r="AU163">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:47">
@@ -23970,7 +23970,7 @@
         <v>102.2</v>
       </c>
       <c r="AU164">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:47">
@@ -24113,7 +24113,7 @@
         <v>85.90000000000001</v>
       </c>
       <c r="AU165">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:47">
@@ -24256,7 +24256,7 @@
         <v>105.1</v>
       </c>
       <c r="AU166">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:47">
@@ -24399,7 +24399,7 @@
         <v>86.59999999999999</v>
       </c>
       <c r="AU167">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:47">
@@ -24542,7 +24542,7 @@
         <v>94.7</v>
       </c>
       <c r="AU168">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:47">
@@ -24685,7 +24685,7 @@
         <v>100.9</v>
       </c>
       <c r="AU169">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:47">
@@ -24828,7 +24828,7 @@
         <v>90.40000000000001</v>
       </c>
       <c r="AU170">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:47">
@@ -24971,7 +24971,7 @@
         <v>105.2</v>
       </c>
       <c r="AU171">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:47">
@@ -25114,7 +25114,7 @@
         <v>114.5</v>
       </c>
       <c r="AU172">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:47">
@@ -25257,7 +25257,7 @@
         <v>97.3</v>
       </c>
       <c r="AU173">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:47">
@@ -25400,7 +25400,7 @@
         <v>100.9</v>
       </c>
       <c r="AU174">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:47">
@@ -25543,7 +25543,7 @@
         <v>97.90000000000001</v>
       </c>
       <c r="AU175">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:47">
@@ -25686,7 +25686,7 @@
         <v>91.59999999999999</v>
       </c>
       <c r="AU176">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:47">
@@ -25829,7 +25829,7 @@
         <v>94.2</v>
       </c>
       <c r="AU177">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:47">
@@ -25972,7 +25972,7 @@
         <v>88.09999999999999</v>
       </c>
       <c r="AU178">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:47">
@@ -26115,7 +26115,7 @@
         <v>126</v>
       </c>
       <c r="AU179">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:47">
@@ -26258,7 +26258,7 @@
         <v>92</v>
       </c>
       <c r="AU180">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:47">
@@ -26401,7 +26401,7 @@
         <v>110.5</v>
       </c>
       <c r="AU181">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:47">
@@ -26544,7 +26544,7 @@
         <v>91.90000000000001</v>
       </c>
       <c r="AU182">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:47">
@@ -26687,7 +26687,7 @@
         <v>115.4</v>
       </c>
       <c r="AU183">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:47">
@@ -26830,7 +26830,7 @@
         <v>105.3</v>
       </c>
       <c r="AU184">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:47">
@@ -26973,7 +26973,7 @@
         <v>105.8</v>
       </c>
       <c r="AU185">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:47">
@@ -27116,7 +27116,7 @@
         <v>121.6</v>
       </c>
       <c r="AU186">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:47">
@@ -27259,7 +27259,7 @@
         <v>114.4</v>
       </c>
       <c r="AU187">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:47">
@@ -27402,7 +27402,7 @@
         <v>107.6</v>
       </c>
       <c r="AU188">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:47">
@@ -27545,7 +27545,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="AU189">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="1:47">
@@ -27688,7 +27688,7 @@
         <v>97.90000000000001</v>
       </c>
       <c r="AU190">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:47">
@@ -27831,7 +27831,7 @@
         <v>102.4</v>
       </c>
       <c r="AU191">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192" spans="1:47">
@@ -27974,7 +27974,7 @@
         <v>103.1</v>
       </c>
       <c r="AU192">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:47">
@@ -28117,7 +28117,7 @@
         <v>105.2</v>
       </c>
       <c r="AU193">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:47">
@@ -28260,7 +28260,7 @@
         <v>112.7</v>
       </c>
       <c r="AU194">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:47">
@@ -28403,7 +28403,7 @@
         <v>118.7</v>
       </c>
       <c r="AU195">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:47">
@@ -28546,7 +28546,7 @@
         <v>113.3</v>
       </c>
       <c r="AU196">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:47">
@@ -28689,7 +28689,7 @@
         <v>86.40000000000001</v>
       </c>
       <c r="AU197">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:47">
@@ -28832,7 +28832,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="AU198">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:47">
@@ -28975,7 +28975,7 @@
         <v>100.9</v>
       </c>
       <c r="AU199">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:47">
@@ -29118,7 +29118,7 @@
         <v>93.59999999999999</v>
       </c>
       <c r="AU200">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:47">
@@ -29261,7 +29261,7 @@
         <v>110.4</v>
       </c>
       <c r="AU201">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202" spans="1:47">
@@ -29404,7 +29404,7 @@
         <v>90</v>
       </c>
       <c r="AU202">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:47">
@@ -29547,7 +29547,7 @@
         <v>94.3</v>
       </c>
       <c r="AU203">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="204" spans="1:47">
@@ -29690,7 +29690,7 @@
         <v>100</v>
       </c>
       <c r="AU204">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:47">
@@ -29833,7 +29833,7 @@
         <v>104.8</v>
       </c>
       <c r="AU205">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:47">
@@ -29976,7 +29976,7 @@
         <v>115.7</v>
       </c>
       <c r="AU206">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="207" spans="1:47">
@@ -30119,7 +30119,7 @@
         <v>91.8</v>
       </c>
       <c r="AU207">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:47">
@@ -30262,7 +30262,7 @@
         <v>106.2</v>
       </c>
       <c r="AU208">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:47">
@@ -30405,7 +30405,7 @@
         <v>106.9</v>
       </c>
       <c r="AU209">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210" spans="1:47">
@@ -30548,7 +30548,7 @@
         <v>107.2</v>
       </c>
       <c r="AU210">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211" spans="1:47">
@@ -30691,7 +30691,7 @@
         <v>88.2</v>
       </c>
       <c r="AU211">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:47">
@@ -30834,7 +30834,7 @@
         <v>143.8</v>
       </c>
       <c r="AU212">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:47">
@@ -30977,7 +30977,7 @@
         <v>99</v>
       </c>
       <c r="AU213">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="214" spans="1:47">
@@ -31120,7 +31120,7 @@
         <v>95.40000000000001</v>
       </c>
       <c r="AU214">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="1:47">
@@ -31263,7 +31263,7 @@
         <v>108.9</v>
       </c>
       <c r="AU215">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="1:47">
@@ -31406,7 +31406,7 @@
         <v>96.8</v>
       </c>
       <c r="AU216">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="217" spans="1:47">
@@ -31549,7 +31549,7 @@
         <v>119.5</v>
       </c>
       <c r="AU217">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:47">
@@ -31692,7 +31692,7 @@
         <v>91.3</v>
       </c>
       <c r="AU218">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:47">
@@ -31835,7 +31835,7 @@
         <v>120.8</v>
       </c>
       <c r="AU219">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:47">
@@ -31978,7 +31978,7 @@
         <v>145.9</v>
       </c>
       <c r="AU220">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:47">
@@ -32121,7 +32121,7 @@
         <v>108.1</v>
       </c>
       <c r="AU221">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:47">
@@ -32264,7 +32264,7 @@
         <v>94.2</v>
       </c>
       <c r="AU222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:47">
@@ -32407,7 +32407,7 @@
         <v>95.90000000000001</v>
       </c>
       <c r="AU223">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:47">
@@ -32550,7 +32550,7 @@
         <v>101.1</v>
       </c>
       <c r="AU224">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="225" spans="1:47">
@@ -32693,7 +32693,7 @@
         <v>103.8</v>
       </c>
       <c r="AU225">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="226" spans="1:47">
@@ -32836,7 +32836,7 @@
         <v>118.9</v>
       </c>
       <c r="AU226">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227" spans="1:47">
@@ -32979,7 +32979,7 @@
         <v>97.59999999999999</v>
       </c>
       <c r="AU227">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228" spans="1:47">
@@ -33122,7 +33122,7 @@
         <v>96</v>
       </c>
       <c r="AU228">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="229" spans="1:47">
@@ -33265,7 +33265,7 @@
         <v>105.9</v>
       </c>
       <c r="AU229">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="230" spans="1:47">
@@ -33408,7 +33408,7 @@
         <v>91.8</v>
       </c>
       <c r="AU230">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231" spans="1:47">
@@ -33551,7 +33551,7 @@
         <v>97.8</v>
       </c>
       <c r="AU231">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:47">
@@ -33694,7 +33694,7 @@
         <v>87.59999999999999</v>
       </c>
       <c r="AU232">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233" spans="1:47">
@@ -33837,7 +33837,7 @@
         <v>118.9</v>
       </c>
       <c r="AU233">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="234" spans="1:47">
@@ -33980,7 +33980,7 @@
         <v>91.3</v>
       </c>
       <c r="AU234">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:47">
@@ -34123,7 +34123,7 @@
         <v>96.40000000000001</v>
       </c>
       <c r="AU235">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="1:47">
@@ -34266,7 +34266,7 @@
         <v>102</v>
       </c>
       <c r="AU236">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237" spans="1:47">
@@ -34409,7 +34409,7 @@
         <v>113.7</v>
       </c>
       <c r="AU237">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:47">
@@ -34552,7 +34552,7 @@
         <v>95.5</v>
       </c>
       <c r="AU238">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="239" spans="1:47">
@@ -34695,7 +34695,7 @@
         <v>94.8</v>
       </c>
       <c r="AU239">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240" spans="1:47">
@@ -34838,7 +34838,7 @@
         <v>85.09999999999999</v>
       </c>
       <c r="AU240">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="241" spans="1:47">
@@ -34981,7 +34981,7 @@
         <v>117.4</v>
       </c>
       <c r="AU241">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="242" spans="1:47">
@@ -35124,7 +35124,7 @@
         <v>103.2</v>
       </c>
       <c r="AU242">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="243" spans="1:47">
@@ -35267,7 +35267,7 @@
         <v>88.59999999999999</v>
       </c>
       <c r="AU243">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="244" spans="1:47">
@@ -35410,7 +35410,7 @@
         <v>107.3</v>
       </c>
       <c r="AU244">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" spans="1:47">
@@ -35553,7 +35553,7 @@
         <v>101.5</v>
       </c>
       <c r="AU245">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246" spans="1:47">
@@ -35696,7 +35696,7 @@
         <v>137.6</v>
       </c>
       <c r="AU246">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="247" spans="1:47">
@@ -35839,7 +35839,7 @@
         <v>101</v>
       </c>
       <c r="AU247">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248" spans="1:47">
@@ -35982,7 +35982,7 @@
         <v>91.8</v>
       </c>
       <c r="AU248">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="249" spans="1:47">
@@ -36125,7 +36125,7 @@
         <v>105.6</v>
       </c>
       <c r="AU249">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="250" spans="1:47">
@@ -36268,7 +36268,7 @@
         <v>97.09999999999999</v>
       </c>
       <c r="AU250">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251" spans="1:47">
@@ -36411,7 +36411,7 @@
         <v>135.6</v>
       </c>
       <c r="AU251">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="252" spans="1:47">
@@ -36554,7 +36554,7 @@
         <v>119.4</v>
       </c>
       <c r="AU252">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253" spans="1:47">
@@ -36697,7 +36697,7 @@
         <v>109.7</v>
       </c>
       <c r="AU253">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="254" spans="1:47">
@@ -36840,7 +36840,7 @@
         <v>112.9</v>
       </c>
       <c r="AU254">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255" spans="1:47">
@@ -36983,7 +36983,7 @@
         <v>99</v>
       </c>
       <c r="AU255">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256" spans="1:47">
@@ -37126,7 +37126,7 @@
         <v>100.4</v>
       </c>
       <c r="AU256">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="257" spans="1:47">
@@ -37269,7 +37269,7 @@
         <v>136.6</v>
       </c>
       <c r="AU257">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="258" spans="1:47">
@@ -37412,7 +37412,7 @@
         <v>90</v>
       </c>
       <c r="AU258">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:47">
@@ -37555,7 +37555,7 @@
         <v>96.3</v>
       </c>
       <c r="AU259">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260" spans="1:47">
@@ -37698,7 +37698,7 @@
         <v>184.1</v>
       </c>
       <c r="AU260">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261" spans="1:47">
@@ -37841,7 +37841,7 @@
         <v>87.40000000000001</v>
       </c>
       <c r="AU261">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="262" spans="1:47">
@@ -37984,7 +37984,7 @@
         <v>94.7</v>
       </c>
       <c r="AU262">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:47">
@@ -38127,7 +38127,7 @@
         <v>142.6</v>
       </c>
       <c r="AU263">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="264" spans="1:47">
@@ -38270,7 +38270,7 @@
         <v>99.09999999999999</v>
       </c>
       <c r="AU264">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="265" spans="1:47">
@@ -38413,7 +38413,7 @@
         <v>110.2</v>
       </c>
       <c r="AU265">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266" spans="1:47">
@@ -38556,7 +38556,7 @@
         <v>93.59999999999999</v>
       </c>
       <c r="AU266">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:47">
@@ -38699,7 +38699,7 @@
         <v>149.3</v>
       </c>
       <c r="AU267">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268" spans="1:47">
@@ -38842,7 +38842,7 @@
         <v>138.9</v>
       </c>
       <c r="AU268">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="269" spans="1:47">
@@ -38985,7 +38985,7 @@
         <v>125.5</v>
       </c>
       <c r="AU269">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="270" spans="1:47">
@@ -39128,7 +39128,7 @@
         <v>107</v>
       </c>
       <c r="AU270">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="271" spans="1:47">
@@ -39271,7 +39271,7 @@
         <v>89.5</v>
       </c>
       <c r="AU271">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="272" spans="1:47">
@@ -39414,7 +39414,7 @@
         <v>118.2</v>
       </c>
       <c r="AU272">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273" spans="1:47">
@@ -39557,7 +39557,7 @@
         <v>134.1</v>
       </c>
       <c r="AU273">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="274" spans="1:47">
@@ -39700,7 +39700,7 @@
         <v>99.5</v>
       </c>
       <c r="AU274">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275" spans="1:47">
@@ -39843,7 +39843,7 @@
         <v>143.5</v>
       </c>
       <c r="AU275">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="276" spans="1:47">
@@ -39986,7 +39986,7 @@
         <v>99.59999999999999</v>
       </c>
       <c r="AU276">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="277" spans="1:47">
@@ -40129,7 +40129,7 @@
         <v>107.5</v>
       </c>
       <c r="AU277">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="278" spans="1:47">
@@ -40272,7 +40272,7 @@
         <v>90.09999999999999</v>
       </c>
       <c r="AU278">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="279" spans="1:47">
@@ -40415,7 +40415,7 @@
         <v>138.3</v>
       </c>
       <c r="AU279">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="280" spans="1:47">
@@ -40558,7 +40558,7 @@
         <v>138.2</v>
       </c>
       <c r="AU280">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" spans="1:47">
@@ -40701,7 +40701,7 @@
         <v>137.7</v>
       </c>
       <c r="AU281">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="282" spans="1:47">
@@ -40844,7 +40844,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="AU282">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:47">
@@ -40987,7 +40987,7 @@
         <v>144.1</v>
       </c>
       <c r="AU283">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="284" spans="1:47">
@@ -41130,7 +41130,7 @@
         <v>128.7</v>
       </c>
       <c r="AU284">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:47">
@@ -41273,7 +41273,7 @@
         <v>116.1</v>
       </c>
       <c r="AU285">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="286" spans="1:47">
@@ -41416,7 +41416,7 @@
         <v>118.1</v>
       </c>
       <c r="AU286">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:47">
@@ -41559,7 +41559,7 @@
         <v>116.7</v>
       </c>
       <c r="AU287">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="288" spans="1:47">
@@ -41702,7 +41702,7 @@
         <v>96.90000000000001</v>
       </c>
       <c r="AU288">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="289" spans="1:47">
@@ -41845,7 +41845,7 @@
         <v>130</v>
       </c>
       <c r="AU289">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290" spans="1:47">
@@ -41988,7 +41988,7 @@
         <v>90.59999999999999</v>
       </c>
       <c r="AU290">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="291" spans="1:47">
@@ -42131,7 +42131,7 @@
         <v>150.8</v>
       </c>
       <c r="AU291">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="292" spans="1:47">
@@ -42274,7 +42274,7 @@
         <v>99.8</v>
       </c>
       <c r="AU292">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="293" spans="1:47">
@@ -42417,7 +42417,7 @@
         <v>121.7</v>
       </c>
       <c r="AU293">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="294" spans="1:47">
@@ -42560,7 +42560,7 @@
         <v>99.59999999999999</v>
       </c>
       <c r="AU294">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="295" spans="1:47">
@@ -42703,7 +42703,7 @@
         <v>132.8</v>
       </c>
       <c r="AU295">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="296" spans="1:47">
@@ -42846,7 +42846,7 @@
         <v>148.6</v>
       </c>
       <c r="AU296">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="297" spans="1:47">
@@ -42989,7 +42989,7 @@
         <v>101</v>
       </c>
       <c r="AU297">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="298" spans="1:47">
@@ -43132,7 +43132,7 @@
         <v>193.1</v>
       </c>
       <c r="AU298">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="299" spans="1:47">
@@ -43275,7 +43275,7 @@
         <v>82.7</v>
       </c>
       <c r="AU299">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300" spans="1:47">
@@ -43418,7 +43418,7 @@
         <v>95.5</v>
       </c>
       <c r="AU300">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="301" spans="1:47">
@@ -43561,7 +43561,7 @@
         <v>119.5</v>
       </c>
       <c r="AU301">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="302" spans="1:47">
@@ -43704,7 +43704,7 @@
         <v>107.9</v>
       </c>
       <c r="AU302">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="303" spans="1:47">
@@ -43847,7 +43847,7 @@
         <v>97.8</v>
       </c>
       <c r="AU303">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="304" spans="1:47">
@@ -43990,7 +43990,7 @@
         <v>104.4</v>
       </c>
       <c r="AU304">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="305" spans="1:47">
@@ -44133,7 +44133,7 @@
         <v>118.5</v>
       </c>
       <c r="AU305">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="306" spans="1:47">
@@ -44276,7 +44276,7 @@
         <v>92.7</v>
       </c>
       <c r="AU306">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="307" spans="1:47">
@@ -44419,7 +44419,7 @@
         <v>115.8</v>
       </c>
       <c r="AU307">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308" spans="1:47">
@@ -44562,7 +44562,7 @@
         <v>115.5</v>
       </c>
       <c r="AU308">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="309" spans="1:47">
@@ -44705,7 +44705,7 @@
         <v>91.8</v>
       </c>
       <c r="AU309">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="310" spans="1:47">
@@ -44848,7 +44848,7 @@
         <v>145.2</v>
       </c>
       <c r="AU310">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="311" spans="1:47">
@@ -44991,7 +44991,7 @@
         <v>109.9</v>
       </c>
       <c r="AU311">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="312" spans="1:47">
@@ -45134,7 +45134,7 @@
         <v>142.9</v>
       </c>
       <c r="AU312">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="313" spans="1:47">
@@ -45277,7 +45277,7 @@
         <v>115.9</v>
       </c>
       <c r="AU313">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314" spans="1:47">
@@ -45420,7 +45420,7 @@
         <v>104.7</v>
       </c>
       <c r="AU314">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="315" spans="1:47">
@@ -45563,7 +45563,7 @@
         <v>92.2</v>
       </c>
       <c r="AU315">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="316" spans="1:47">
@@ -45706,7 +45706,7 @@
         <v>113.5</v>
       </c>
       <c r="AU316">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:47">
@@ -45849,7 +45849,7 @@
         <v>102.1</v>
       </c>
       <c r="AU317">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318" spans="1:47">
@@ -45992,7 +45992,7 @@
         <v>210.6</v>
       </c>
       <c r="AU318">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="319" spans="1:47">
@@ -46135,7 +46135,7 @@
         <v>99.8</v>
       </c>
       <c r="AU319">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" spans="1:47">
@@ -46278,7 +46278,7 @@
         <v>123.4</v>
       </c>
       <c r="AU320">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>